<commit_message>
3rd Commit with validating homepage and selecting flights page
</commit_message>
<xml_diff>
--- a/YatraAutomation/src/test/resources/testData/cityinput.xlsx
+++ b/YatraAutomation/src/test/resources/testData/cityinput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14265" windowHeight="4890"/>
+    <workbookView windowWidth="15570" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>hyderabad</t>
   </si>
@@ -34,14 +34,20 @@
   <si>
     <t>jabalpur</t>
   </si>
+  <si>
+    <t>BLR</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -54,6 +60,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -78,6 +92,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,39 +121,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,8 +144,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,14 +162,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,181 +219,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,15 +431,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -449,15 +446,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -469,6 +457,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,6 +487,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -503,15 +509,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -521,130 +527,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -971,13 +977,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="10.2857142857143" customWidth="1"/>
   </cols>
@@ -1014,6 +1020,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>